<commit_message>
Update 20170927 01 Cập nhật yêu cầu hệ thống
</commit_message>
<xml_diff>
--- a/Yeu-cau/YeuCau.xlsx
+++ b/Yeu-cau/YeuCau.xlsx
@@ -479,6 +479,93 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -518,93 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -959,60 +959,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="D11" s="5">
         <f ca="1">IF(A11="","", NOW())</f>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D12" s="5">
         <f t="shared" ref="D12:D75" ca="1" si="1">IF(A12="","", NOW())</f>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="D14" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D15" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D16" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="D17" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>43005.701009375</v>
+        <v>43005.702136689812</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="11" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="11" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
@@ -1974,25 +1974,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="29" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" style="29" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="19" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -2001,1947 +2001,1947 @@
       <c r="A2" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+    <row r="12" spans="1:10" s="11" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
         <f>IF(B12="", "", IF(A11="STT", 1, A12+1))</f>
         <v>1</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="28">
         <f ca="1">IF(A12="","",TODAY())</f>
         <v>43005</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+    <row r="13" spans="1:10" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
         <f>IF(B13="", "", IF(A12="STT", 1, A12+1))</f>
         <v>2</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="28">
         <f t="shared" ref="D13:D77" ca="1" si="0">IF(A13="","",TODAY())</f>
         <v>43005</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+    <row r="14" spans="1:10" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
         <f t="shared" ref="A14:A78" si="1">IF(B14="", "", IF(A13="STT", 1, A13+1))</f>
         <v>3</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37" t="s">
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36">
+    <row r="15" spans="1:10" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37" t="s">
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="36">
+    <row r="16" spans="1:10" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="21" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
+    <row r="17" spans="1:7" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37" t="s">
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="21" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36">
+    <row r="18" spans="1:7" s="11" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
         <f t="shared" ref="A18:A27" si="2">IF(B18="", "", IF(A17="STT", 1, A17+1))</f>
         <v>7</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="28">
         <f t="shared" ref="D18" ca="1" si="3">IF(A18="","",TODAY())</f>
         <v>43005</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
+    <row r="19" spans="1:7" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="31" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="39">
+    <row r="20" spans="1:7" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40" t="s">
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+    <row r="21" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40" t="s">
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="31" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+    <row r="22" spans="1:7" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="31" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+    <row r="23" spans="1:7" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40" t="s">
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="31" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+    <row r="24" spans="1:7" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40" t="s">
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="31" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="39">
+    <row r="25" spans="1:7" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40" t="s">
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="31" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
+    <row r="26" spans="1:7" s="21" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="41">
+      <c r="D26" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40" t="s">
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="39">
+    <row r="27" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40" t="s">
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+    <row r="28" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44" t="s">
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
+    <row r="29" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="33">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="45">
+      <c r="D29" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44" t="s">
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+    <row r="30" spans="1:7" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="45">
+      <c r="D30" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44" t="s">
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="43">
+    <row r="31" spans="1:7" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44" t="s">
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="32" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43">
+    <row r="32" spans="1:7" s="22" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="43">
+    <row r="33" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44" t="s">
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+    <row r="34" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="45">
+      <c r="D34" s="35">
         <f t="shared" ca="1" si="0"/>
         <v>43005</v>
       </c>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44" t="s">
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35" t="str">
+      <c r="A35" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="24" t="str">
+      <c r="A36" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="24" t="str">
+      <c r="A37" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="24" t="str">
+      <c r="A38" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="24" t="str">
+      <c r="A39" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="24" t="str">
+      <c r="A40" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="24" t="str">
+      <c r="A41" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="F42" s="42"/>
+      <c r="A42" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="24" t="str">
+      <c r="A43" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="24" t="str">
+      <c r="A44" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="24" t="str">
+      <c r="A45" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="24" t="str">
+      <c r="A46" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="24" t="str">
+      <c r="A47" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="24" t="str">
+      <c r="A48" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="24" t="str">
+      <c r="A49" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="24" t="str">
+      <c r="A50" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="24" t="str">
+      <c r="A51" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="24" t="str">
+      <c r="A52" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="24" t="str">
+      <c r="A53" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="24" t="str">
+      <c r="A54" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="24" t="str">
+      <c r="A55" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="24" t="str">
+      <c r="A56" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="24" t="str">
+      <c r="A57" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="24" t="str">
+      <c r="A58" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="24" t="str">
+      <c r="A59" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="24" t="str">
+      <c r="A60" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="24" t="str">
+      <c r="A61" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="24" t="str">
+      <c r="A62" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="24" t="str">
+      <c r="A63" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="24" t="str">
+      <c r="A64" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="24" t="str">
+      <c r="A65" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="24" t="str">
+      <c r="A66" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="24" t="str">
+      <c r="A67" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="24" t="str">
+      <c r="A68" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="24" t="str">
+      <c r="A69" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="24" t="str">
+      <c r="A70" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="24" t="str">
+      <c r="A71" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="24" t="str">
+      <c r="A72" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="24" t="str">
+      <c r="A73" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="24" t="str">
+      <c r="A74" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B75" s="28"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="24" t="str">
+      <c r="A75" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B76" s="28"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="24" t="str">
+      <c r="A76" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B77" s="28"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="24" t="str">
+      <c r="A77" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="14" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B78" s="28"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="24" t="str">
+      <c r="A78" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="14" t="str">
         <f t="shared" ref="D78:D101" ca="1" si="4">IF(A78="","",TODAY())</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="str">
+      <c r="A79" s="12" t="str">
         <f t="shared" ref="A79:A101" si="5">IF(B79="", "", IF(A78="STT", 1, A78+1))</f>
         <v/>
       </c>
-      <c r="B79" s="28"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="24" t="str">
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="22" t="str">
+      <c r="A80" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B80" s="28"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="24" t="str">
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="str">
+      <c r="A81" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="24" t="str">
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="str">
+      <c r="A82" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B82" s="28"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="24" t="str">
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="str">
+      <c r="A83" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="24" t="str">
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="str">
+      <c r="A84" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="24" t="str">
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="str">
+      <c r="A85" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="24" t="str">
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="22" t="str">
+      <c r="A86" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="24" t="str">
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="str">
+      <c r="A87" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="24" t="str">
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="str">
+      <c r="A88" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B88" s="28"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="24" t="str">
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="str">
+      <c r="A89" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B89" s="28"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="24" t="str">
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="22" t="str">
+      <c r="A90" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="24" t="str">
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="str">
+      <c r="A91" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="24" t="str">
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="22" t="str">
+      <c r="A92" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="24" t="str">
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="22" t="str">
+      <c r="A93" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="24" t="str">
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="22" t="str">
+      <c r="A94" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="24" t="str">
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="22" t="str">
+      <c r="A95" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="24" t="str">
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="22" t="str">
+      <c r="A96" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="24" t="str">
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="22" t="str">
+      <c r="A97" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="24" t="str">
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="22" t="str">
+      <c r="A98" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="24" t="str">
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="22" t="str">
+      <c r="A99" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B99" s="28"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="24" t="str">
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="str">
+      <c r="A100" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="24" t="str">
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="22" t="str">
+      <c r="A101" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="24" t="str">
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="23"/>
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="25"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="15"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="23"/>
-      <c r="B103" s="28"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="25"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="15"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
-      <c r="B104" s="28"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="25"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="15"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="23"/>
-      <c r="B105" s="28"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="25"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="15"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
-      <c r="B106" s="28"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="25"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="15"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="23"/>
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="25"/>
+      <c r="A107" s="13"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="15"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
-      <c r="B108" s="28"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="25"/>
+      <c r="A108" s="13"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="15"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="23"/>
-      <c r="B109" s="28"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="25"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="15"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="23"/>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="25"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="15"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="23"/>
-      <c r="B111" s="28"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="25"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="15"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="23"/>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="25"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="15"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="23"/>
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="25"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="15"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="23"/>
-      <c r="B114" s="28"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="25"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="15"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="23"/>
-      <c r="B115" s="28"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="25"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="15"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="23"/>
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="25"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="15"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="23"/>
-      <c r="B117" s="28"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="25"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="15"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="23"/>
-      <c r="B118" s="28"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="25"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="15"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="23"/>
-      <c r="B119" s="28"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="25"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="15"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="23"/>
-      <c r="B120" s="28"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="25"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="18"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="15"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
-      <c r="B121" s="28"/>
-      <c r="C121" s="28"/>
-      <c r="D121" s="25"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="15"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="23"/>
-      <c r="B122" s="28"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="25"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="15"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="23"/>
-      <c r="B123" s="28"/>
-      <c r="C123" s="28"/>
-      <c r="D123" s="25"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="18"/>
+      <c r="C123" s="18"/>
+      <c r="D123" s="15"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
-      <c r="B124" s="28"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="25"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="18"/>
+      <c r="C124" s="18"/>
+      <c r="D124" s="15"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="23"/>
-      <c r="B125" s="28"/>
-      <c r="C125" s="28"/>
-      <c r="D125" s="25"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="18"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="15"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="23"/>
-      <c r="B126" s="28"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="25"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="18"/>
+      <c r="C126" s="18"/>
+      <c r="D126" s="15"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="23"/>
-      <c r="B127" s="28"/>
-      <c r="C127" s="28"/>
-      <c r="D127" s="25"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="15"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="23"/>
-      <c r="B128" s="28"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="25"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="18"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="15"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="23"/>
-      <c r="B129" s="28"/>
-      <c r="C129" s="28"/>
-      <c r="D129" s="25"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="15"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="23"/>
-      <c r="B130" s="28"/>
-      <c r="C130" s="28"/>
-      <c r="D130" s="25"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="18"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="15"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="23"/>
-      <c r="B131" s="28"/>
-      <c r="C131" s="28"/>
-      <c r="D131" s="25"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="18"/>
+      <c r="C131" s="18"/>
+      <c r="D131" s="15"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="23"/>
-      <c r="B132" s="28"/>
-      <c r="C132" s="28"/>
-      <c r="D132" s="25"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="18"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="15"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="23"/>
-      <c r="B133" s="28"/>
-      <c r="C133" s="28"/>
-      <c r="D133" s="25"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="18"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="15"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="23"/>
-      <c r="B134" s="28"/>
-      <c r="C134" s="28"/>
-      <c r="D134" s="25"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="18"/>
+      <c r="C134" s="18"/>
+      <c r="D134" s="15"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="23"/>
-      <c r="B135" s="28"/>
-      <c r="C135" s="28"/>
-      <c r="D135" s="25"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="18"/>
+      <c r="C135" s="18"/>
+      <c r="D135" s="15"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="23"/>
-      <c r="B136" s="28"/>
-      <c r="C136" s="28"/>
-      <c r="D136" s="25"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="15"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="23"/>
-      <c r="B137" s="28"/>
-      <c r="C137" s="28"/>
-      <c r="D137" s="25"/>
+      <c r="A137" s="13"/>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="15"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="23"/>
-      <c r="B138" s="28"/>
-      <c r="C138" s="28"/>
-      <c r="D138" s="25"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="15"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="23"/>
-      <c r="B139" s="28"/>
-      <c r="C139" s="28"/>
-      <c r="D139" s="25"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="18"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="15"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="23"/>
-      <c r="B140" s="28"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="25"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="18"/>
+      <c r="C140" s="18"/>
+      <c r="D140" s="15"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="23"/>
-      <c r="B141" s="28"/>
-      <c r="C141" s="28"/>
-      <c r="D141" s="25"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="18"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="15"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="23"/>
-      <c r="B142" s="28"/>
-      <c r="C142" s="28"/>
-      <c r="D142" s="25"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="18"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="15"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="23"/>
-      <c r="B143" s="28"/>
-      <c r="C143" s="28"/>
-      <c r="D143" s="25"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="18"/>
+      <c r="C143" s="18"/>
+      <c r="D143" s="15"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="23"/>
-      <c r="B144" s="28"/>
-      <c r="C144" s="28"/>
-      <c r="D144" s="25"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="18"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="15"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="23"/>
-      <c r="B145" s="28"/>
-      <c r="C145" s="28"/>
-      <c r="D145" s="25"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="18"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="15"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="23"/>
-      <c r="B146" s="28"/>
-      <c r="C146" s="28"/>
-      <c r="D146" s="25"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="18"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="15"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="23"/>
-      <c r="B147" s="28"/>
-      <c r="C147" s="28"/>
-      <c r="D147" s="25"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="18"/>
+      <c r="C147" s="18"/>
+      <c r="D147" s="15"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="23"/>
-      <c r="B148" s="28"/>
-      <c r="C148" s="28"/>
-      <c r="D148" s="25"/>
+      <c r="A148" s="13"/>
+      <c r="B148" s="18"/>
+      <c r="C148" s="18"/>
+      <c r="D148" s="15"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="23"/>
-      <c r="B149" s="28"/>
-      <c r="C149" s="28"/>
-      <c r="D149" s="25"/>
+      <c r="A149" s="13"/>
+      <c r="B149" s="18"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="15"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="23"/>
-      <c r="B150" s="28"/>
-      <c r="C150" s="28"/>
-      <c r="D150" s="25"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="18"/>
+      <c r="C150" s="18"/>
+      <c r="D150" s="15"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="23"/>
-      <c r="B151" s="28"/>
-      <c r="C151" s="28"/>
-      <c r="D151" s="25"/>
+      <c r="A151" s="13"/>
+      <c r="B151" s="18"/>
+      <c r="C151" s="18"/>
+      <c r="D151" s="15"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="23"/>
-      <c r="B152" s="28"/>
-      <c r="C152" s="28"/>
-      <c r="D152" s="25"/>
+      <c r="A152" s="13"/>
+      <c r="B152" s="18"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="15"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="23"/>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="25"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="18"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="15"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="23"/>
-      <c r="B154" s="28"/>
-      <c r="C154" s="28"/>
-      <c r="D154" s="25"/>
+      <c r="A154" s="13"/>
+      <c r="B154" s="18"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="15"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="23"/>
-      <c r="B155" s="28"/>
-      <c r="C155" s="28"/>
-      <c r="D155" s="25"/>
+      <c r="A155" s="13"/>
+      <c r="B155" s="18"/>
+      <c r="C155" s="18"/>
+      <c r="D155" s="15"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="23"/>
-      <c r="B156" s="28"/>
-      <c r="C156" s="28"/>
-      <c r="D156" s="25"/>
+      <c r="A156" s="13"/>
+      <c r="B156" s="18"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="15"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="23"/>
-      <c r="B157" s="28"/>
-      <c r="C157" s="28"/>
-      <c r="D157" s="25"/>
+      <c r="A157" s="13"/>
+      <c r="B157" s="18"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="15"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="23"/>
-      <c r="B158" s="28"/>
-      <c r="C158" s="28"/>
-      <c r="D158" s="25"/>
+      <c r="A158" s="13"/>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="15"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="23"/>
-      <c r="B159" s="28"/>
-      <c r="C159" s="28"/>
-      <c r="D159" s="25"/>
+      <c r="A159" s="13"/>
+      <c r="B159" s="18"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="15"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="23"/>
-      <c r="B160" s="28"/>
-      <c r="C160" s="28"/>
-      <c r="D160" s="25"/>
+      <c r="A160" s="13"/>
+      <c r="B160" s="18"/>
+      <c r="C160" s="18"/>
+      <c r="D160" s="15"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="23"/>
-      <c r="B161" s="28"/>
-      <c r="C161" s="28"/>
-      <c r="D161" s="25"/>
+      <c r="A161" s="13"/>
+      <c r="B161" s="18"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="15"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="23"/>
-      <c r="B162" s="28"/>
-      <c r="C162" s="28"/>
-      <c r="D162" s="25"/>
+      <c r="A162" s="13"/>
+      <c r="B162" s="18"/>
+      <c r="C162" s="18"/>
+      <c r="D162" s="15"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="23"/>
-      <c r="B163" s="28"/>
-      <c r="C163" s="28"/>
-      <c r="D163" s="25"/>
+      <c r="A163" s="13"/>
+      <c r="B163" s="18"/>
+      <c r="C163" s="18"/>
+      <c r="D163" s="15"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="23"/>
-      <c r="B164" s="28"/>
-      <c r="C164" s="28"/>
-      <c r="D164" s="25"/>
+      <c r="A164" s="13"/>
+      <c r="B164" s="18"/>
+      <c r="C164" s="18"/>
+      <c r="D164" s="15"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="23"/>
-      <c r="B165" s="28"/>
-      <c r="C165" s="28"/>
-      <c r="D165" s="25"/>
+      <c r="A165" s="13"/>
+      <c r="B165" s="18"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="15"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="23"/>
-      <c r="B166" s="28"/>
-      <c r="C166" s="28"/>
-      <c r="D166" s="25"/>
+      <c r="A166" s="13"/>
+      <c r="B166" s="18"/>
+      <c r="C166" s="18"/>
+      <c r="D166" s="15"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="23"/>
-      <c r="B167" s="28"/>
-      <c r="C167" s="28"/>
-      <c r="D167" s="25"/>
+      <c r="A167" s="13"/>
+      <c r="B167" s="18"/>
+      <c r="C167" s="18"/>
+      <c r="D167" s="15"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="23"/>
-      <c r="B168" s="28"/>
-      <c r="C168" s="28"/>
-      <c r="D168" s="25"/>
+      <c r="A168" s="13"/>
+      <c r="B168" s="18"/>
+      <c r="C168" s="18"/>
+      <c r="D168" s="15"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="23"/>
-      <c r="B169" s="28"/>
-      <c r="C169" s="28"/>
-      <c r="D169" s="25"/>
+      <c r="A169" s="13"/>
+      <c r="B169" s="18"/>
+      <c r="C169" s="18"/>
+      <c r="D169" s="15"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="23"/>
-      <c r="B170" s="28"/>
-      <c r="C170" s="28"/>
-      <c r="D170" s="25"/>
+      <c r="A170" s="13"/>
+      <c r="B170" s="18"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="15"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="23"/>
-      <c r="B171" s="28"/>
-      <c r="C171" s="28"/>
-      <c r="D171" s="25"/>
+      <c r="A171" s="13"/>
+      <c r="B171" s="18"/>
+      <c r="C171" s="18"/>
+      <c r="D171" s="15"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="23"/>
-      <c r="B172" s="28"/>
-      <c r="C172" s="28"/>
-      <c r="D172" s="25"/>
+      <c r="A172" s="13"/>
+      <c r="B172" s="18"/>
+      <c r="C172" s="18"/>
+      <c r="D172" s="15"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="23"/>
-      <c r="B173" s="28"/>
-      <c r="C173" s="28"/>
-      <c r="D173" s="25"/>
+      <c r="A173" s="13"/>
+      <c r="B173" s="18"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="15"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="23"/>
-      <c r="B174" s="28"/>
-      <c r="C174" s="28"/>
-      <c r="D174" s="25"/>
-      <c r="E174" s="30"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="18"/>
+      <c r="C174" s="18"/>
+      <c r="D174" s="15"/>
+      <c r="E174" s="20"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="23"/>
-      <c r="B175" s="28"/>
-      <c r="C175" s="28"/>
-      <c r="D175" s="25"/>
+      <c r="A175" s="13"/>
+      <c r="B175" s="18"/>
+      <c r="C175" s="18"/>
+      <c r="D175" s="15"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="23"/>
-      <c r="B176" s="28"/>
-      <c r="C176" s="28"/>
-      <c r="D176" s="25"/>
+      <c r="A176" s="13"/>
+      <c r="B176" s="18"/>
+      <c r="C176" s="18"/>
+      <c r="D176" s="15"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="23"/>
-      <c r="B177" s="28"/>
-      <c r="C177" s="28"/>
-      <c r="D177" s="25"/>
+      <c r="A177" s="13"/>
+      <c r="B177" s="18"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="15"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="23"/>
-      <c r="B178" s="28"/>
-      <c r="C178" s="28"/>
-      <c r="D178" s="25"/>
+      <c r="A178" s="13"/>
+      <c r="B178" s="18"/>
+      <c r="C178" s="18"/>
+      <c r="D178" s="15"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="23"/>
-      <c r="B179" s="28"/>
-      <c r="C179" s="28"/>
-      <c r="D179" s="25"/>
+      <c r="A179" s="13"/>
+      <c r="B179" s="18"/>
+      <c r="C179" s="18"/>
+      <c r="D179" s="15"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="23"/>
-      <c r="B180" s="28"/>
-      <c r="C180" s="28"/>
-      <c r="D180" s="25"/>
+      <c r="A180" s="13"/>
+      <c r="B180" s="18"/>
+      <c r="C180" s="18"/>
+      <c r="D180" s="15"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="23"/>
-      <c r="B181" s="28"/>
-      <c r="C181" s="28"/>
-      <c r="D181" s="25"/>
+      <c r="A181" s="13"/>
+      <c r="B181" s="18"/>
+      <c r="C181" s="18"/>
+      <c r="D181" s="15"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="23"/>
-      <c r="B182" s="28"/>
-      <c r="C182" s="28"/>
-      <c r="D182" s="25"/>
+      <c r="A182" s="13"/>
+      <c r="B182" s="18"/>
+      <c r="C182" s="18"/>
+      <c r="D182" s="15"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="23"/>
-      <c r="B183" s="28"/>
-      <c r="C183" s="28"/>
-      <c r="D183" s="25"/>
+      <c r="A183" s="13"/>
+      <c r="B183" s="18"/>
+      <c r="C183" s="18"/>
+      <c r="D183" s="15"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="23"/>
-      <c r="B184" s="28"/>
-      <c r="C184" s="28"/>
-      <c r="D184" s="25"/>
+      <c r="A184" s="13"/>
+      <c r="B184" s="18"/>
+      <c r="C184" s="18"/>
+      <c r="D184" s="15"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="23"/>
-      <c r="B185" s="28"/>
-      <c r="C185" s="28"/>
-      <c r="D185" s="25"/>
+      <c r="A185" s="13"/>
+      <c r="B185" s="18"/>
+      <c r="C185" s="18"/>
+      <c r="D185" s="15"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="23"/>
-      <c r="B186" s="28"/>
-      <c r="C186" s="28"/>
-      <c r="D186" s="25"/>
+      <c r="A186" s="13"/>
+      <c r="B186" s="18"/>
+      <c r="C186" s="18"/>
+      <c r="D186" s="15"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="23"/>
-      <c r="B187" s="28"/>
-      <c r="C187" s="28"/>
-      <c r="D187" s="25"/>
+      <c r="A187" s="13"/>
+      <c r="B187" s="18"/>
+      <c r="C187" s="18"/>
+      <c r="D187" s="15"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="23"/>
-      <c r="B188" s="28"/>
-      <c r="C188" s="28"/>
-      <c r="D188" s="25"/>
+      <c r="A188" s="13"/>
+      <c r="B188" s="18"/>
+      <c r="C188" s="18"/>
+      <c r="D188" s="15"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="23"/>
-      <c r="B189" s="28"/>
-      <c r="C189" s="28"/>
-      <c r="D189" s="25"/>
+      <c r="A189" s="13"/>
+      <c r="B189" s="18"/>
+      <c r="C189" s="18"/>
+      <c r="D189" s="15"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="23"/>
-      <c r="B190" s="28"/>
-      <c r="C190" s="28"/>
-      <c r="D190" s="25"/>
+      <c r="A190" s="13"/>
+      <c r="B190" s="18"/>
+      <c r="C190" s="18"/>
+      <c r="D190" s="15"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="23"/>
-      <c r="B191" s="28"/>
-      <c r="C191" s="28"/>
-      <c r="D191" s="25"/>
+      <c r="A191" s="13"/>
+      <c r="B191" s="18"/>
+      <c r="C191" s="18"/>
+      <c r="D191" s="15"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="23"/>
-      <c r="B192" s="28"/>
-      <c r="C192" s="28"/>
-      <c r="D192" s="25"/>
+      <c r="A192" s="13"/>
+      <c r="B192" s="18"/>
+      <c r="C192" s="18"/>
+      <c r="D192" s="15"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="23"/>
-      <c r="B193" s="28"/>
-      <c r="C193" s="28"/>
-      <c r="D193" s="25"/>
+      <c r="A193" s="13"/>
+      <c r="B193" s="18"/>
+      <c r="C193" s="18"/>
+      <c r="D193" s="15"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="23"/>
-      <c r="B194" s="28"/>
-      <c r="C194" s="28"/>
-      <c r="D194" s="25"/>
+      <c r="A194" s="13"/>
+      <c r="B194" s="18"/>
+      <c r="C194" s="18"/>
+      <c r="D194" s="15"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="23"/>
-      <c r="B195" s="28"/>
-      <c r="C195" s="28"/>
-      <c r="D195" s="25"/>
+      <c r="A195" s="13"/>
+      <c r="B195" s="18"/>
+      <c r="C195" s="18"/>
+      <c r="D195" s="15"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="23"/>
-      <c r="B196" s="28"/>
-      <c r="C196" s="28"/>
-      <c r="D196" s="25"/>
+      <c r="A196" s="13"/>
+      <c r="B196" s="18"/>
+      <c r="C196" s="18"/>
+      <c r="D196" s="15"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="23"/>
-      <c r="B197" s="28"/>
-      <c r="C197" s="28"/>
-      <c r="D197" s="25"/>
+      <c r="A197" s="13"/>
+      <c r="B197" s="18"/>
+      <c r="C197" s="18"/>
+      <c r="D197" s="15"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="23"/>
-      <c r="B198" s="28"/>
-      <c r="C198" s="28"/>
-      <c r="D198" s="25"/>
+      <c r="A198" s="13"/>
+      <c r="B198" s="18"/>
+      <c r="C198" s="18"/>
+      <c r="D198" s="15"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="23"/>
-      <c r="B199" s="28"/>
-      <c r="C199" s="28"/>
-      <c r="D199" s="25"/>
+      <c r="A199" s="13"/>
+      <c r="B199" s="18"/>
+      <c r="C199" s="18"/>
+      <c r="D199" s="15"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="23"/>
-      <c r="B200" s="28"/>
-      <c r="C200" s="28"/>
-      <c r="D200" s="25"/>
+      <c r="A200" s="13"/>
+      <c r="B200" s="18"/>
+      <c r="C200" s="18"/>
+      <c r="D200" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>